<commit_message>
revise power flow model
</commit_message>
<xml_diff>
--- a/data/Vietanm_electricity_statistics.xlsx
+++ b/data/Vietanm_electricity_statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\mye500\projects\Map2Grid\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF54CEA-49D4-4D4B-A554-70BBB01A26FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD427A85-F2E6-47C1-9F38-063F4BF503AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1526" yWindow="10183" windowWidth="19543" windowHeight="12377" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1526" yWindow="10183" windowWidth="19543" windowHeight="12377" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Installed_capacity" sheetId="1" r:id="rId1"/>
@@ -949,7 +949,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1913,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7F0D24-CCF2-4A85-8875-2CE1DB07434F}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2946,8 +2946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13558E2-00A1-4977-A88F-59E267D57995}">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3408,7 +3408,7 @@
         <v>66</v>
       </c>
       <c r="C18" s="12">
-        <f>I18/$I$80*$C$80</f>
+        <f t="shared" ref="C18:C40" si="0">I18/$I$80*$C$80</f>
         <v>17667.596425966785</v>
       </c>
       <c r="D18" s="4">
@@ -3438,7 +3438,7 @@
         <v>67</v>
       </c>
       <c r="C19" s="12">
-        <f>I19/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>4255.0298829907761</v>
       </c>
       <c r="D19" s="4">
@@ -3468,7 +3468,7 @@
         <v>68</v>
       </c>
       <c r="C20" s="12">
-        <f>I20/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>241.69078558094094</v>
       </c>
       <c r="D20" s="4">
@@ -3498,7 +3498,7 @@
         <v>69</v>
       </c>
       <c r="C21" s="12">
-        <f>I21/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>8423.5599058788994</v>
       </c>
       <c r="D21" s="4">
@@ -3528,7 +3528,7 @@
         <v>70</v>
       </c>
       <c r="C22" s="12">
-        <f>I22/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>4117.6477522395044</v>
       </c>
       <c r="D22" s="4">
@@ -3558,7 +3558,7 @@
         <v>71</v>
       </c>
       <c r="C23" s="12">
-        <f>I23/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>4509.4412362338717</v>
       </c>
       <c r="D23" s="4">
@@ -3588,7 +3588,7 @@
         <v>72</v>
       </c>
       <c r="C24" s="12">
-        <f>I24/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>6093.1519101721424</v>
       </c>
       <c r="D24" s="4">
@@ -3618,7 +3618,7 @@
         <v>73</v>
       </c>
       <c r="C25" s="12">
-        <f>I25/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>3788.1850497896953</v>
       </c>
       <c r="D25" s="4">
@@ -3648,7 +3648,7 @@
         <v>74</v>
       </c>
       <c r="C26" s="12">
-        <f>I26/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>454.12426553892584</v>
       </c>
       <c r="D26" s="4">
@@ -3678,7 +3678,7 @@
         <v>75</v>
       </c>
       <c r="C27" s="12">
-        <f>I27/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>231.51433145121709</v>
       </c>
       <c r="D27" s="4">
@@ -3708,7 +3708,7 @@
         <v>76</v>
       </c>
       <c r="C28" s="12">
-        <f>I28/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>2823.9660209983626</v>
       </c>
       <c r="D28" s="4">
@@ -3738,7 +3738,7 @@
         <v>77</v>
       </c>
       <c r="C29" s="12">
-        <f>I29/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>9717.2416371200416</v>
       </c>
       <c r="D29" s="4">
@@ -3768,7 +3768,7 @@
         <v>78</v>
       </c>
       <c r="C30" s="12">
-        <f>I30/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>14496.358907791593</v>
       </c>
       <c r="D30" s="4">
@@ -3798,7 +3798,7 @@
         <v>79</v>
       </c>
       <c r="C31" s="12">
-        <f>I31/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>10902.798543232866</v>
       </c>
       <c r="D31" s="4">
@@ -3828,7 +3828,7 @@
         <v>80</v>
       </c>
       <c r="C32" s="12">
-        <f>I32/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>11009.651311594967</v>
       </c>
       <c r="D32" s="4">
@@ -3858,7 +3858,7 @@
         <v>81</v>
       </c>
       <c r="C33" s="12">
-        <f>I33/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>2077.2686992298763</v>
       </c>
       <c r="D33" s="4">
@@ -3888,7 +3888,7 @@
         <v>82</v>
       </c>
       <c r="C34" s="12">
-        <f>I34/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>3325.1563868872609</v>
       </c>
       <c r="D34" s="4">
@@ -3918,7 +3918,7 @@
         <v>83</v>
       </c>
       <c r="C35" s="12">
-        <f>I35/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>8474.4421765275183</v>
       </c>
       <c r="D35" s="4">
@@ -3948,7 +3948,7 @@
         <v>84</v>
       </c>
       <c r="C36" s="12">
-        <f>I36/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>1152.4834301912235</v>
       </c>
       <c r="D36" s="4">
@@ -3978,7 +3978,7 @@
         <v>85</v>
       </c>
       <c r="C37" s="12">
-        <f>I37/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>465.57277643486515</v>
       </c>
       <c r="D37" s="4">
@@ -4008,7 +4008,7 @@
         <v>86</v>
       </c>
       <c r="C38" s="12">
-        <f>I38/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>962.94697202511725</v>
       </c>
       <c r="D38" s="4">
@@ -4038,7 +4038,7 @@
         <v>87</v>
       </c>
       <c r="C39" s="12">
-        <f>I39/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>465.57277643486515</v>
       </c>
       <c r="D39" s="4">
@@ -4068,7 +4068,7 @@
         <v>88</v>
       </c>
       <c r="C40" s="12">
-        <f>I40/$I$80*$C$80</f>
+        <f t="shared" si="0"/>
         <v>933.68966640216138</v>
       </c>
       <c r="D40" s="4">
@@ -4433,7 +4433,7 @@
         <v>102</v>
       </c>
       <c r="C55" s="16">
-        <f>I55/$I$80*$C$80</f>
+        <f t="shared" ref="C55:C60" si="1">I55/$I$80*$C$80</f>
         <v>2252.8125329676127</v>
       </c>
       <c r="D55" s="4">
@@ -4463,7 +4463,7 @@
         <v>103</v>
       </c>
       <c r="C56" s="16">
-        <f>I56/$I$80*$C$80</f>
+        <f t="shared" si="1"/>
         <v>628.39604251044636</v>
       </c>
       <c r="D56" s="4">
@@ -4493,7 +4493,7 @@
         <v>104</v>
       </c>
       <c r="C57" s="16">
-        <f>I57/$I$80*$C$80</f>
+        <f t="shared" si="1"/>
         <v>480.83745762945091</v>
       </c>
       <c r="D57" s="4">
@@ -4523,7 +4523,7 @@
         <v>105</v>
       </c>
       <c r="C58" s="16">
-        <f>I58/$I$80*$C$80</f>
+        <f t="shared" si="1"/>
         <v>93061.128902791985</v>
       </c>
       <c r="D58" s="6">
@@ -4553,7 +4553,7 @@
         <v>106</v>
       </c>
       <c r="C59" s="16">
-        <f>I59/$I$80*$C$80</f>
+        <f t="shared" si="1"/>
         <v>2447.4372181985809</v>
       </c>
       <c r="D59">
@@ -4583,7 +4583,7 @@
         <v>107</v>
       </c>
       <c r="C60" s="16">
-        <f>I60/$I$80*$C$80</f>
+        <f t="shared" si="1"/>
         <v>2893.9291431402139</v>
       </c>
       <c r="D60">
@@ -5127,8 +5127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB65EAF5-A56E-4270-8472-89080845ECB0}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>